<commit_message>
Testes com hospitalização - Argentina
</commit_message>
<xml_diff>
--- a/Parameters_Rosario.xlsx
+++ b/Parameters_Rosario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,16 +468,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2146</v>
+        <v>1948</v>
       </c>
       <c r="D2" t="n">
-        <v>219</v>
+        <v>76</v>
       </c>
       <c r="E2" t="n">
-        <v>0.265</v>
+        <v>0.1</v>
       </c>
       <c r="F2" t="n">
-        <v>22.7</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="3">
@@ -488,16 +488,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>415</v>
+        <v>3342</v>
       </c>
       <c r="D3" t="n">
-        <v>328</v>
+        <v>217</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1</v>
+        <v>0.244</v>
       </c>
       <c r="F3" t="n">
-        <v>21.8</v>
+        <v>33.2</v>
       </c>
     </row>
     <row r="4">
@@ -508,16 +508,56 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
+        <v>689</v>
+      </c>
+      <c r="D4" t="n">
+        <v>324</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
         <v>1736</v>
       </c>
-      <c r="D4" t="n">
-        <v>453</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.407</v>
-      </c>
-      <c r="F4" t="n">
-        <v>25.3</v>
+      <c r="D5" t="n">
+        <v>418</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2068</v>
+      </c>
+      <c r="D6" t="n">
+        <v>490</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>40.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>